<commit_message>
Ajuste de vista en Excel
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (Maestral)/Documentos/Clases/UC - Web scrapping/web_scraping_soc40XX/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA6FCFA-9561-FA43-A5B7-7C603B20196F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897584D6-6B62-F64C-A8DD-B358C49FEBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2300" windowWidth="29020" windowHeight="17440" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6AE771-24D7-9544-8CD7-00832CCAF6F4}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualización links en calendario.
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (Maestral)/Documentos/Clases/UC - Web scrapping/web_scraping_soc40XX/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897584D6-6B62-F64C-A8DD-B358C49FEBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF2AABC-C4DA-7C47-B337-639C610B2141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2300" windowWidth="29020" windowHeight="17440" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>tipo</t>
   </si>
@@ -127,7 +127,10 @@
     <t>[Slides](slides/class_3/class_3#1) [.Rmd](slides/class_3/class_3.Rmd)</t>
   </si>
   <si>
-    <t>[Slides](slides/class_2/class_2#1) [.Rmd](slides/class_4/class_4.Rmd) [.R](slides/class_4/class_4_taller.R)</t>
+    <t>[Slides](slides/class_5/class_5#1) [.Rmd](slides/class_5/class_5.Rmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_4/class_2#1) [.Rmd](slides/class_4/class_4.Rmd) [.R](slides/class_4/class_4_taller.R)</t>
   </si>
 </sst>
 </file>
@@ -496,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6AE771-24D7-9544-8CD7-00832CCAF6F4}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -634,6 +637,9 @@
       </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>